<commit_message>
Added resume in excel
</commit_message>
<xml_diff>
--- a/Resumen_Slope_And_BPoints.xlsx
+++ b/Resumen_Slope_And_BPoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -278,22 +278,28 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +605,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G20" sqref="G20"/>
+      <selection pane="topRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,53 +615,53 @@
   <sheetData>
     <row r="1" spans="1:39" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5" t="s">
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
     </row>
-    <row r="2" spans="1:39" s="10" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:39" s="7" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -736,7 +742,7 @@
       <c r="AM2" s="9"/>
     </row>
     <row r="3" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -853,7 +859,7 @@
       </c>
     </row>
     <row r="4" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="1">
@@ -892,39 +898,95 @@
       <c r="M4" s="1">
         <v>2.7900999999999998</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
       <c r="D5" s="2">
         <v>-3.1850999999999998</v>
       </c>
@@ -949,8 +1011,12 @@
       <c r="K5" s="2">
         <v>0.4103</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
       <c r="N5" s="2">
         <v>-2.7008999999999999</v>
       </c>
@@ -963,35 +1029,83 @@
       <c r="Q5" s="2">
         <v>3.6299000000000001</v>
       </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="2"/>
-      <c r="AM5" s="2"/>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
       <c r="D6" s="1">
         <v>-2.5817999999999999</v>
       </c>
@@ -1016,41 +1130,93 @@
       <c r="K6" s="1">
         <v>9.0374999999999996</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
       <c r="R6" s="1">
         <v>-11.189</v>
       </c>
       <c r="S6" s="1">
         <v>9.0374999999999996</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2">
@@ -1083,37 +1249,93 @@
       <c r="K7" s="2">
         <v>4.8044000000000002</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12">
+        <v>0</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12">
+        <v>0</v>
+      </c>
+      <c r="V7" s="12">
+        <v>0</v>
+      </c>
+      <c r="W7" s="12">
+        <v>0</v>
+      </c>
+      <c r="X7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1">
@@ -1146,37 +1368,93 @@
       <c r="K8" s="1">
         <v>7.5292000000000003</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
-      <c r="AM8" s="1"/>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="2">
@@ -1209,37 +1487,93 @@
       <c r="K9" s="2">
         <v>9.9239999999999995</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="1">
@@ -1272,41 +1606,101 @@
       <c r="K10" s="1">
         <v>4.7575000000000003</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
       <c r="D11" s="2">
         <v>-2.2534999999999998</v>
       </c>
@@ -1325,59 +1719,155 @@
       <c r="I11" s="2">
         <v>2.827</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="2"/>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:39" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
       <c r="T12" s="1">
         <v>-2.7244999999999999</v>
       </c>
@@ -1396,31 +1886,71 @@
       <c r="Y12" s="1">
         <v>1.6455</v>
       </c>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1"/>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
       <c r="H13" s="2">
         <v>-2.7267999999999999</v>
       </c>
@@ -1433,20 +1963,48 @@
       <c r="K13" s="2">
         <v>1.8627</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
       <c r="Z13" s="2">
         <v>-3.2818999999999998</v>
       </c>
@@ -1471,49 +2029,125 @@
       <c r="AG13" s="2">
         <v>1.0175000000000001</v>
       </c>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
+      <c r="AH13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>0</v>
+      </c>
       <c r="AH14" s="1">
         <v>-2.3542999999999998</v>
       </c>
@@ -1534,7 +2168,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="2">
@@ -1543,8 +2177,12 @@
       <c r="C15" s="2">
         <v>3.0886</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
       <c r="F15" s="2">
         <v>-1.6554</v>
       </c>
@@ -1563,40 +2201,102 @@
       <c r="K15" s="2">
         <v>5.6744000000000003</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="1"/>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2">
+        <v>0</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="S1:AD1"/>
@@ -1613,12 +2313,6 @@
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>